<commit_message>
Completed Stats Module 2
</commit_message>
<xml_diff>
--- a/2. Stats Essentials/2.Investment Assignment/Investments.xlsx
+++ b/2. Stats Essentials/2.Investment Assignment/Investments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/demon/Documents/upgrad/ai-ml/2. Stats Essentials/2.Investment Assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5162902B-AAB7-3B4B-9110-BCAC0B89840D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC65FC0B-9070-684F-BEB3-015B3E69E3D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table -1.1" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="60">
   <si>
     <t>C1</t>
   </si>
@@ -361,13 +361,74 @@
   </si>
   <si>
     <t>permalink</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Venture</t>
+  </si>
+  <si>
+    <t>United States of America (USA)</t>
+  </si>
+  <si>
+    <t>India ( IND)</t>
+  </si>
+  <si>
+    <t>United Kingdom(GBR)</t>
+  </si>
+  <si>
+    <t>108,531,347,515 USD</t>
+  </si>
+  <si>
+    <t>5,436,843,539 USD</t>
+  </si>
+  <si>
+    <t>2,976,543,602 USD</t>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <t>Social, Finance, Analytics, Advertising</t>
+  </si>
+  <si>
+    <t>Cleantech / Semiconductors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Social, Finance, Analytics, Advertising	</t>
+  </si>
+  <si>
+    <t>News, Search and Messaging</t>
+  </si>
+  <si>
+    <t>Virtustream</t>
+  </si>
+  <si>
+    <t>Electric Cloud</t>
+  </si>
+  <si>
+    <t>FirstCry.com</t>
+  </si>
+  <si>
+    <t>Celltick Technologies</t>
+  </si>
+  <si>
+    <t>SST Inc. (Formerly ShotSpotter)</t>
+  </si>
+  <si>
+    <t>Manthan Systems</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -435,6 +496,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -574,10 +649,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -591,17 +667,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -619,14 +689,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -645,11 +708,32 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -678,8 +762,10 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -994,8 +1080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1006,91 +1092,95 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="15"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="22"/>
     </row>
     <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="15"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="22"/>
     </row>
     <row r="3" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
+      <c r="A5" s="21">
         <v>1</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="10">
         <v>66373</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
+      <c r="A6" s="21">
         <v>2</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="10">
         <v>66368</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
+      <c r="A7" s="21">
         <v>3</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="10" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="5">
+      <c r="A8" s="21">
         <v>4</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="17"/>
+      <c r="C8" s="10" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="5">
+      <c r="A9" s="21">
         <v>5</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="17"/>
+      <c r="C9" s="10">
+        <v>114949</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="11"/>
+      <c r="B10" s="9"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="11"/>
+      <c r="B11" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1116,7 +1206,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1127,77 +1217,87 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="27"/>
+      <c r="B1" s="29"/>
     </row>
     <row r="2" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
     </row>
     <row r="3" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
     </row>
     <row r="4" spans="1:3" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="12">
+      <c r="A5" s="10">
         <v>1</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="12"/>
+      <c r="C5" s="25">
+        <v>5000000</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="12">
+      <c r="A6" s="10">
         <v>2</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="12"/>
+      <c r="C6" s="25">
+        <v>400000</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="12">
+      <c r="A7" s="10">
         <v>3</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="12"/>
+      <c r="C7" s="25">
+        <v>275000</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="12">
+      <c r="A8" s="10">
         <v>4</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="12"/>
+      <c r="C8" s="25">
+        <v>20000000</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="12">
+      <c r="A9" s="10">
         <v>5</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="12"/>
+      <c r="C9" s="26" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1224,70 +1324,76 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.1640625" customWidth="1"/>
     <col min="2" max="2" width="47.1640625" customWidth="1"/>
-    <col min="3" max="3" width="21.5" customWidth="1"/>
+    <col min="3" max="3" width="24.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="27"/>
+      <c r="B1" s="29"/>
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
     </row>
     <row r="3" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="7" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>1</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="6"/>
+      <c r="C5" s="5" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A6" s="6">
+      <c r="A6" s="5">
         <v>2</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C6" s="5" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A7" s="6">
+      <c r="A7" s="5">
         <v>3</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="5" t="s">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1310,166 +1416,227 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="1"/>
     <col min="2" max="2" width="56.83203125" customWidth="1"/>
-    <col min="3" max="3" width="17.5" customWidth="1"/>
-    <col min="4" max="4" width="14.83203125" customWidth="1"/>
-    <col min="5" max="5" width="17.1640625" customWidth="1"/>
+    <col min="3" max="5" width="29.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="31"/>
+      <c r="B1" s="33"/>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="32"/>
-      <c r="B2" s="33"/>
+      <c r="A2" s="34"/>
+      <c r="B2" s="35"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="19" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="19">
+      <c r="A5" s="14">
         <v>1</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
+      <c r="C5" s="13">
+        <v>12150</v>
+      </c>
+      <c r="D5" s="13">
+        <v>628</v>
+      </c>
+      <c r="E5" s="13">
+        <v>330</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="19">
+      <c r="A6" s="14">
         <v>2</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
+      <c r="C6" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="19">
+      <c r="A7" s="14">
         <v>3</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
+      <c r="C7" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="19">
+      <c r="A8" s="14">
         <v>4</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
+      <c r="C8" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="19">
+      <c r="A9" s="14">
         <v>5</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
+      <c r="C9" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="19">
+      <c r="A10" s="14">
         <v>6</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
+      <c r="C10" s="13">
+        <v>2950</v>
+      </c>
+      <c r="D10" s="13">
+        <v>147</v>
+      </c>
+      <c r="E10" s="13">
+        <v>110</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="19">
+      <c r="A11" s="14">
         <v>7</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
+      <c r="C11" s="13">
+        <v>2714</v>
+      </c>
+      <c r="D11" s="13">
+        <v>130</v>
+      </c>
+      <c r="E11" s="13">
+        <v>60</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="19">
+      <c r="A12" s="14">
         <v>8</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
+      <c r="C12" s="13">
+        <v>2350</v>
+      </c>
+      <c r="D12" s="13">
+        <v>133</v>
+      </c>
+      <c r="E12" s="13">
+        <v>52</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A13" s="19">
+      <c r="A13" s="14">
         <v>9</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
+      <c r="C13" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="14" spans="1:5" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="19">
+      <c r="A14" s="14">
         <v>10</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
+      <c r="C14" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="C15" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>